<commit_message>
Save imported file accounts
</commit_message>
<xml_diff>
--- a/src/assets/data/chart-accounts/plantillaCatalogoCuentas.xlsx
+++ b/src/assets/data/chart-accounts/plantillaCatalogoCuentas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naren\OneDrive\Desktop\Naren Unicauca\OCTAVO SEMESTRE\Proyecto I\C2\frontend\frontend_accounting_software\src\assets\data\chart-accounts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fre90\Desktop\frontend_accounting_software\src\assets\data\chart-accounts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B3162A4-D8C2-4BEE-84E3-EB24BB3758C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ECC9835-9608-400A-A70C-C2E0D69EB56E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="69">
   <si>
     <t>Código</t>
   </si>
@@ -44,6 +44,102 @@
     <t>Nombre</t>
   </si>
   <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>1105</t>
+  </si>
+  <si>
+    <t>Efectivo y equivalentes de efectivo</t>
+  </si>
+  <si>
+    <t>110501</t>
+  </si>
+  <si>
+    <t>11050101</t>
+  </si>
+  <si>
+    <t>Caja principal</t>
+  </si>
+  <si>
+    <t>11050102</t>
+  </si>
+  <si>
+    <t>110502</t>
+  </si>
+  <si>
+    <t>1106</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>1205</t>
+  </si>
+  <si>
+    <t>Propiedades, planta y equipo</t>
+  </si>
+  <si>
+    <t>1206</t>
+  </si>
+  <si>
+    <t>Activos intangibles</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Pasivos</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>2105</t>
+  </si>
+  <si>
+    <t>Cuentas por pagar</t>
+  </si>
+  <si>
+    <t>2106</t>
+  </si>
+  <si>
+    <t>Obligaciones financieras corrientes</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>2205</t>
+  </si>
+  <si>
+    <t>Obligaciones financieras no corrientes</t>
+  </si>
+  <si>
+    <t>2206</t>
+  </si>
+  <si>
+    <t>Beneficios a empleados a largo plazo</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>Utilidades acumuladas</t>
+  </si>
+  <si>
+    <t>Utilidades NO acumuladas</t>
+  </si>
+  <si>
     <t>Naturaleza</t>
   </si>
   <si>
@@ -96,6 +192,57 @@
   </si>
   <si>
     <t>Ingresos No Operacionales</t>
+  </si>
+  <si>
+    <t>Activos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patrimonio </t>
+  </si>
+  <si>
+    <t>Ingresos</t>
+  </si>
+  <si>
+    <t>Gastos</t>
+  </si>
+  <si>
+    <t>Costos de ventas</t>
+  </si>
+  <si>
+    <t>Costos de transformación</t>
+  </si>
+  <si>
+    <t>Cuentas de orden deudoras</t>
+  </si>
+  <si>
+    <t>Cuentas de orden acreedoras</t>
+  </si>
+  <si>
+    <t>Inversiones e instrumentos derivados</t>
+  </si>
+  <si>
+    <t>Operaciones de banca central e instituciones financieras</t>
+  </si>
+  <si>
+    <t>Emisión y colocación de títulos de deuda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Capital social </t>
+  </si>
+  <si>
+    <t>Caja</t>
+  </si>
+  <si>
+    <t>Caja menor</t>
+  </si>
+  <si>
+    <t>Reservas internacionales</t>
+  </si>
+  <si>
+    <t>Banco menor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Banco </t>
   </si>
 </sst>
 </file>
@@ -518,24 +665,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.75" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="39.19921875" customWidth="1"/>
-    <col min="3" max="3" width="16.09765625" customWidth="1"/>
-    <col min="4" max="4" width="26.796875" customWidth="1"/>
-    <col min="5" max="5" width="26.296875" customWidth="1"/>
-    <col min="6" max="6" width="16.796875" customWidth="1"/>
+    <col min="2" max="2" width="39.25" customWidth="1"/>
+    <col min="3" max="3" width="16.125" customWidth="1"/>
+    <col min="4" max="4" width="26.75" customWidth="1"/>
+    <col min="5" max="5" width="26.25" customWidth="1"/>
+    <col min="6" max="6" width="16.75" customWidth="1"/>
     <col min="7" max="7" width="28.5" customWidth="1"/>
     <col min="8" max="8" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -543,231 +690,559 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="B2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
+      <c r="B4" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>45</v>
+      </c>
       <c r="F4" s="2"/>
       <c r="H4" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="H5" s="2" t="s">
+      <c r="B11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="H6" s="2" t="s">
+      <c r="B12" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="H7" s="2" t="s">
+      <c r="C12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="H8" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="H9" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="H11" s="1"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
+      <c r="B14" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>33</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>4</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>5</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>6</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>7</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>8</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>9</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Seleccione una opcion" sqref="C2:C23" xr:uid="{3301FE25-B2F6-4E95-AD01-C7E26F351373}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Seleccione una opcion" sqref="C2:C29" xr:uid="{3301FE25-B2F6-4E95-AD01-C7E26F351373}">
       <formula1>$F$2:$F$3</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D23" xr:uid="{5ACFD159-61F2-4A64-9D7A-698FA311E28F}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D29" xr:uid="{5ACFD159-61F2-4A64-9D7A-698FA311E28F}">
       <formula1>$G$2:$G$3</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E23" xr:uid="{362A2C83-B6A2-4429-9532-2BF21E03128B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E29" xr:uid="{362A2C83-B6A2-4429-9532-2BF21E03128B}">
       <formula1>$H$2:$H$9</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:B1" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:B1 A6 A2 A3 A22:B22 A20 A21 A9 A7 A11:B13 A10 A15:B16 A14 A18:B19 A17 A4 A5 A8" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>